<commit_message>
Payment with Card Test Cases completed
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="1300" yWindow="3680" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>sac@grr.la</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>sac15@grr.la</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>0222</t>
   </si>
 </sst>
 </file>
@@ -100,9 +106,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -437,14 +444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
@@ -496,6 +504,14 @@
       </c>
       <c r="B3" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CMS Test Case Done
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="3680" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>sac@grr.la</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>0222</t>
+  </si>
+  <si>
+    <t>CMS Username</t>
+  </si>
+  <si>
+    <t>CMS Password</t>
+  </si>
+  <si>
+    <t>Vamsi</t>
+  </si>
+  <si>
+    <t>Vamsi123*</t>
   </si>
 </sst>
 </file>
@@ -444,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -512,6 +524,22 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Successfully completed MGC P0 Test Cases
</commit_message>
<xml_diff>
--- a/input/data.xlsx
+++ b/input/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>sac@grr.la</t>
   </si>
@@ -117,21 +117,6 @@
     <t>Paypal new Registered email id</t>
   </si>
   <si>
-    <t>sac70@grr.la</t>
-  </si>
-  <si>
-    <t>sac71@grr.la</t>
-  </si>
-  <si>
-    <t>sac72@grr.la</t>
-  </si>
-  <si>
-    <t>sac73@grr.la</t>
-  </si>
-  <si>
-    <t>sac74@grr.la</t>
-  </si>
-  <si>
     <t>Relative jpg path</t>
   </si>
   <si>
@@ -157,6 +142,24 @@
   </si>
   <si>
     <t>/Users/sachin/eclipse-workspace/MGC_Auto/input/Sample.pdf</t>
+  </si>
+  <si>
+    <t>sac80@grr.la</t>
+  </si>
+  <si>
+    <t>sac81@grr.la</t>
+  </si>
+  <si>
+    <t>sac82@grr.la</t>
+  </si>
+  <si>
+    <t>sac83@grr.la</t>
+  </si>
+  <si>
+    <t>sac84@grr.la</t>
+  </si>
+  <si>
+    <t>sac85@grr.la</t>
   </si>
 </sst>
 </file>
@@ -578,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -601,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -624,13 +627,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -714,13 +720,13 @@
         <v>29</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="90">
@@ -743,22 +749,22 @@
         <v>2</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -769,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -792,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
@@ -815,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -856,6 +862,7 @@
     <hyperlink ref="C17" r:id="rId5"/>
     <hyperlink ref="C18" r:id="rId6"/>
     <hyperlink ref="A21" r:id="rId7"/>
+    <hyperlink ref="G2" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>